<commit_message>
Add New Template Files and Dummy datas
</commit_message>
<xml_diff>
--- a/dummy_data.xlsx
+++ b/dummy_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -34,10 +34,7 @@
     <t xml:space="preserve">end date</t>
   </si>
   <si>
-    <t xml:space="preserve">vivek shree unikrishan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EYEQ202504215</t>
+    <t xml:space="preserve">Johnson powder boi</t>
   </si>
   <si>
     <t xml:space="preserve">21-02-2025</t>
@@ -49,9 +46,6 @@
     <t xml:space="preserve">adam</t>
   </si>
   <si>
-    <t xml:space="preserve">EYEQ202504216</t>
-  </si>
-  <si>
     <t xml:space="preserve">21-02-2026</t>
   </si>
   <si>
@@ -61,9 +55,6 @@
     <t xml:space="preserve">eve</t>
   </si>
   <si>
-    <t xml:space="preserve">EYEQ202504217</t>
-  </si>
-  <si>
     <t xml:space="preserve">21-02-2027</t>
   </si>
   <si>
@@ -71,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">rahul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EYEQ202504218</t>
   </si>
   <si>
     <t xml:space="preserve">21-02-2028</t>
@@ -289,7 +277,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -312,56 +300,56 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1" t="n">
+        <v>202504215</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>202504216</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>202504217</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="1" t="n">
+        <v>202504218</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Custom font func, add bold font file and causing some error so reverting to old commit for now
</commit_message>
<xml_diff>
--- a/dummy_data.xlsx
+++ b/dummy_data.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">end date</t>
   </si>
   <si>
-    <t xml:space="preserve">Johnson powder boi</t>
+    <t xml:space="preserve">Johnson P A powder boi</t>
   </si>
   <si>
     <t xml:space="preserve">21-02-2025</t>
@@ -277,7 +277,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Enhance CertificateApp UI and functionality: updated title to "CertWizard", improved navigation and button styling, added modern status and info displays, and refined certificate generation process. Removed outdated project files and updated project file extensions to .certwiz.
</commit_message>
<xml_diff>
--- a/dummy_data.xlsx
+++ b/dummy_data.xlsx
@@ -20,21 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end date</t>
+  </si>
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Johnson P A powder boi</t>
+    <t xml:space="preserve">123@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">21-02-2025</t>
@@ -43,31 +46,43 @@
     <t xml:space="preserve">21-03-2025</t>
   </si>
   <si>
+    <t xml:space="preserve">Johnson powder boi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">124@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-02-2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-03-2026</t>
+  </si>
+  <si>
     <t xml:space="preserve">adam</t>
   </si>
   <si>
-    <t xml:space="preserve">21-02-2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2026</t>
+    <t xml:space="preserve">125@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-02-2027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-03-2027</t>
   </si>
   <si>
     <t xml:space="preserve">eve</t>
   </si>
   <si>
-    <t xml:space="preserve">21-02-2027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2027</t>
+    <t xml:space="preserve">126@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-02-2028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21-03-2028</t>
   </si>
   <si>
     <t xml:space="preserve">rahul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-02-2028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21-03-2028</t>
   </si>
 </sst>
 </file>
@@ -77,7 +92,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -98,6 +113,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -142,12 +164,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -274,13 +300,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.95"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -295,64 +324,82 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>202504215</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>202504216</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>202504217</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>202504218</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="123@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>